<commit_message>
Fix issue with 0201 components in the BOM file (0603 were chosen by jlcpcb auto tool by default).
</commit_message>
<xml_diff>
--- a/picoamp-straddle-usbc/jlcpcb/nextpcb-bom.xlsx
+++ b/picoamp-straddle-usbc/jlcpcb/nextpcb-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teigue\projects\picoamp-PCB\picoamp-straddle-usbc\jlcpcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC137D5-B2C7-48BC-A03D-C4A7D26B8551}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5D042F-1E44-42B7-BFBE-1FE1052836D9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="4440" windowHeight="1630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>FootPrint</t>
   </si>
@@ -40,27 +40,15 @@
     <t>C129131</t>
   </si>
   <si>
-    <t>CC0603KRX7R9BB104</t>
-  </si>
-  <si>
     <t>C12,C14,C15,C17,C19,C20,C21,C22,C23,C24</t>
   </si>
   <si>
     <t>0603</t>
   </si>
   <si>
-    <t>C14663</t>
-  </si>
-  <si>
-    <t>CL10C150JB8NNNC</t>
-  </si>
-  <si>
     <t>C5,C6</t>
   </si>
   <si>
-    <t>C1644</t>
-  </si>
-  <si>
     <t>CL10A106KP8NNNC</t>
   </si>
   <si>
@@ -82,30 +70,12 @@
     <t>C2040</t>
   </si>
   <si>
-    <t>0603WAF1001T5E</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>C21190</t>
-  </si>
-  <si>
-    <t>0603WAF5101T5E</t>
-  </si>
-  <si>
-    <t>C23186</t>
-  </si>
-  <si>
-    <t>0603WAF270JT5E</t>
-  </si>
-  <si>
     <t>R2,R3</t>
   </si>
   <si>
-    <t>C25190</t>
-  </si>
-  <si>
     <t>W25Q16JVUXIQ</t>
   </si>
   <si>
@@ -203,6 +173,39 @@
   </si>
   <si>
     <t>ship waste qty with the order pls</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
+    <t>0201X104M100CT</t>
+  </si>
+  <si>
+    <t>C2443222</t>
+  </si>
+  <si>
+    <t>RTT0127R0FTH</t>
+  </si>
+  <si>
+    <t>C158649</t>
+  </si>
+  <si>
+    <t>RM02F5101CT</t>
+  </si>
+  <si>
+    <t>C4153144</t>
+  </si>
+  <si>
+    <t>WR02X102JAL</t>
+  </si>
+  <si>
+    <t>C170199</t>
+  </si>
+  <si>
+    <t>RF03N150F250CT</t>
+  </si>
+  <si>
+    <t>C3896518</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -303,6 +306,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +638,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -633,13 +651,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="33">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -648,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -668,287 +686,287 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
+      <c r="D4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
+      <c r="A7" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
+      <c r="A8" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
+      <c r="A9" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5">

</xml_diff>